<commit_message>
Run weekly profitability analysis for Long and Short reversal strategies - Aug 2, 2025
</commit_message>
<xml_diff>
--- a/Daily/analysis/Weekly_Reports/short_weekly_breakdown_summary.xlsx
+++ b/Daily/analysis/Weekly_Reports/short_weekly_breakdown_summary.xlsx
@@ -61,6 +61,9 @@
     <t>Week 1</t>
   </si>
   <si>
+    <t>Jul 26 - Aug 01</t>
+  </si>
+  <si>
     <t>Jul 19 - Jul 25</t>
   </si>
   <si>
@@ -70,31 +73,28 @@
     <t>Jul 05 - Jul 11</t>
   </si>
   <si>
-    <t>Jun 28 - Jul 04</t>
+    <t>PEL</t>
   </si>
   <si>
     <t>SWANENERGY</t>
   </si>
   <si>
-    <t>ATUL</t>
+    <t>SWSOLAR</t>
   </si>
   <si>
     <t>MOTHERSON</t>
   </si>
   <si>
-    <t>CONCOR</t>
-  </si>
-  <si>
-    <t>HAPPYFORGE</t>
-  </si>
-  <si>
-    <t>JINDALSTEL</t>
+    <t>OPTIEMUS</t>
+  </si>
+  <si>
+    <t>VISHNU</t>
+  </si>
+  <si>
+    <t>JIOFIN</t>
   </si>
   <si>
     <t>ANANDRATHI</t>
-  </si>
-  <si>
-    <t>JGCHEM</t>
   </si>
 </sst>
 </file>
@@ -501,31 +501,31 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>79.54545454545455</v>
+        <v>78.94736842105263</v>
       </c>
       <c r="G2">
-        <v>1.929304601018013</v>
+        <v>1.693924098935704</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2">
-        <v>6.977886977886978</v>
+        <v>7.688155459592847</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
       <c r="K2">
-        <v>-2.022400339720787</v>
+        <v>-4.393214441061331</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -536,31 +536,31 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>71.66666666666667</v>
+        <v>87.71929824561403</v>
       </c>
       <c r="G3">
-        <v>1.920431780246215</v>
+        <v>3.66457762960062</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
       </c>
       <c r="I3">
-        <v>10.93447331507581</v>
+        <v>12.82555282555282</v>
       </c>
       <c r="J3" t="s">
         <v>24</v>
       </c>
       <c r="K3">
-        <v>-7.485222998387961</v>
+        <v>-7.584830339321358</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -571,31 +571,31 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E4">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>71.95121951219512</v>
+        <v>83.11688311688312</v>
       </c>
       <c r="G4">
-        <v>1.874706897155071</v>
+        <v>4.705261222161528</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
       </c>
       <c r="I4">
-        <v>35.23526754017944</v>
+        <v>16.49961449498844</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
       <c r="K4">
-        <v>-22.16448580471443</v>
+        <v>-4.272151898734177</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -606,31 +606,31 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="D5">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F5">
-        <v>58.87850467289719</v>
+        <v>76.92307692307693</v>
       </c>
       <c r="G5">
-        <v>0.8736927006894537</v>
+        <v>3.602457862903674</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
       </c>
       <c r="I5">
-        <v>19.91831815747188</v>
+        <v>38.33344090879752</v>
       </c>
       <c r="J5" t="s">
         <v>26</v>
       </c>
       <c r="K5">
-        <v>-19.175</v>
+        <v>-22.94392744106948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>